<commit_message>
Update for GRDevDay, 2018-06.
</commit_message>
<xml_diff>
--- a/Async Languages/Async in Languages.xlsx
+++ b/Async Languages/Async in Languages.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Presentations\Async Languages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F5EFE88F-811E-4682-907A-F6AD2C44BFC9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIOBE" sheetId="2" r:id="rId1"/>
     <sheet name="PYPL" sheetId="3" r:id="rId2"/>
-    <sheet name="Aug 2017" sheetId="1" r:id="rId3"/>
-    <sheet name="Jan 2016" sheetId="4" r:id="rId4"/>
+    <sheet name="June 2018" sheetId="5" r:id="rId3"/>
+    <sheet name="Aug 2017" sheetId="1" r:id="rId4"/>
+    <sheet name="Jan 2016" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>Java</t>
   </si>
@@ -70,11 +72,17 @@
   <si>
     <t>Perl</t>
   </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Matlab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +438,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Aug 2017'!$A$1:$A$10</c:f>
+              <c:f>'June 2018'!$A$1:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -455,10 +463,10 @@
                   <c:v>PHP</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Ruby</c:v>
+                  <c:v>SQL</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Perl</c:v>
+                  <c:v>R</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>C</c:v>
@@ -468,39 +476,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Aug 2017'!$B$1:$B$10</c:f>
+              <c:f>'June 2018'!$B$1:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.1950000000000003</c:v>
+                  <c:v>4.3140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.569</c:v>
+                  <c:v>3.762</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6920000000000002</c:v>
+                  <c:v>5.7610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0979999999999999</c:v>
+                  <c:v>2.4950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.55</c:v>
+                  <c:v>8.3369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.961</c:v>
+                  <c:v>15.368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2930000000000001</c:v>
+                  <c:v>2.8809999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9650000000000001</c:v>
+                  <c:v>2.339</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9950000000000001</c:v>
+                  <c:v>1.452</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4770000000000003</c:v>
+                  <c:v>14.936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,7 +798,7 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2">
-                  <a:lumMod val="50000"/>
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -864,7 +872,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Aug 2017'!$A$12:$A$21</c:f>
+              <c:f>'June 2018'!$A$12:$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -895,46 +903,46 @@
                   <c:v>R</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>C</c:v>
+                  <c:v>Matlab</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Aug 2017'!$B$12:$B$21</c:f>
+              <c:f>'June 2018'!$B$12:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.3</c:v>
+                  <c:v>23.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6</c:v>
+                  <c:v>6.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.7</c:v>
+                  <c:v>22.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9</c:v>
+                  <c:v>8.2100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6</c:v>
+                  <c:v>3.46</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6</c:v>
+                  <c:v>4.1399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4</c:v>
+                  <c:v>2.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1557,10 +1565,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="149" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1568,10 +1576,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1582,7 +1590,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8674782" cy="6296728"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1615,7 +1623,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8664222" cy="6286500"/>
+    <xdr:ext cx="8674782" cy="6296728"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1906,7 +1914,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AC4CF9-C52F-4EE1-8ED1-B34FEF3B4A64}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>4.3140000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>3.762</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5.7610000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2.4950000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>8.3369999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>15.368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2.8809999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>2.339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1.452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>14.936</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>23.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>22.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>2.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2083,8 +2269,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>